<commit_message>
Flow excel files are updated
</commit_message>
<xml_diff>
--- a/android/flow-android.xlsx
+++ b/android/flow-android.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utetsuo/workplace/amazonpay-webviewapp-sample-v2/android/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utetsuo/workplace/amazonpay-sample-app-v2/android/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643D71E6-D9C6-E849-A6B5-2876B5082341}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F9DE1D-E9AD-444B-B078-6A61BED606FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4720" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{31041FA4-F250-5B48-8777-A21A45303114}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>にアクセス</t>
   </si>
@@ -66,12 +66,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>裏で本物のAmazonPayボタンを</t>
-  </si>
-  <si>
-    <t>を指定して、自動的にClick。</t>
-  </si>
-  <si>
     <t>https://10.0.2.2:3443/sample/cart</t>
   </si>
   <si>
@@ -88,6 +82,9 @@
   </si>
   <si>
     <t>https://10.0.2.2:3443/sample/checkoutReview?amazonCheckoutSessionId={id}</t>
+  </si>
+  <si>
+    <t>自動的にLogin画面に遷移</t>
   </si>
 </sst>
 </file>
@@ -4900,7 +4897,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCEA858D-4327-E246-AC75-10AD98E76650}">
   <dimension ref="B1:BE58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7486,7 +7485,7 @@
       <c r="B46" s="15"/>
       <c r="C46" s="23"/>
       <c r="D46" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -7620,7 +7619,7 @@
       <c r="P48" s="10"/>
       <c r="Q48" s="10"/>
       <c r="R48" s="10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="S48" s="5"/>
       <c r="T48" s="10"/>
@@ -7679,9 +7678,7 @@
       <c r="O49" s="3"/>
       <c r="P49" s="18"/>
       <c r="Q49" s="3"/>
-      <c r="R49" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="R49" s="3"/>
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
@@ -7738,7 +7735,7 @@
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
       <c r="N50" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
@@ -7759,7 +7756,7 @@
       <c r="AE50" s="5"/>
       <c r="AF50" s="5"/>
       <c r="AG50" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AH50" s="5"/>
       <c r="AK50" s="5"/>
@@ -7769,7 +7766,7 @@
       <c r="AO50" s="5"/>
       <c r="AP50" s="5"/>
       <c r="AQ50" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AR50" s="5"/>
       <c r="AS50" s="5"/>
@@ -7779,7 +7776,7 @@
       <c r="AW50" s="5"/>
       <c r="AX50" s="5"/>
       <c r="AY50" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AZ50" s="5"/>
       <c r="BA50" s="5"/>
@@ -7835,7 +7832,7 @@
       <c r="AO51" s="5"/>
       <c r="AP51" s="5"/>
       <c r="AQ51" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AR51" s="5"/>
       <c r="AS51" s="5"/>

</xml_diff>

<commit_message>
add document about fixed signature pattern
</commit_message>
<xml_diff>
--- a/android/flow-android.xlsx
+++ b/android/flow-android.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utetsuo/workplace/amazonpay-sample-app-v2/android/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F9DE1D-E9AD-444B-B078-6A61BED606FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDA5F27-3D7A-9C41-B865-46EE3E3C3CE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4720" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{31041FA4-F250-5B48-8777-A21A45303114}"/>
+    <workbookView xWindow="-2860" yWindow="-28740" windowWidth="51400" windowHeight="24300" xr2:uid="{31041FA4-F250-5B48-8777-A21A45303114}"/>
   </bookViews>
   <sheets>
     <sheet name="flow" sheetId="4" r:id="rId1"/>
+    <sheet name="flow-fixed-signature" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
   <si>
     <t>にアクセス</t>
   </si>
@@ -4598,6 +4599,1354 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rounded Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B99C6E6-E53F-F34B-8521-1A96BD18EB48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11391900" y="2286000"/>
+          <a:ext cx="15773400" cy="7289800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-JP" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Secure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>WebView</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>52173</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3F22507-48DB-3146-A6D2-AE6E281EEA93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15392400" y="3022600"/>
+          <a:ext cx="3822700" cy="6198973"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>34668</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A6E132D-9FEB-7646-AF31-1C876478D953}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11595100" y="2984500"/>
+          <a:ext cx="3835400" cy="6219568"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>117274</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>65502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371730</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>61846</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="U-Turn Arrow 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8166938B-7D1B-0B4C-B821-63D386B35888}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="8620063">
+          <a:off x="14150774" y="8828502"/>
+          <a:ext cx="1079956" cy="605944"/>
+        </a:xfrm>
+        <a:prstGeom prst="uturnArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E01AAAA3-88E3-6B4C-B4BD-32F88B0E8EF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14846300" y="6045200"/>
+          <a:ext cx="800100" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46E62F5C-84E7-014C-8566-3F4B6A4025D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7785100" y="698500"/>
+          <a:ext cx="1930400" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>&lt;App&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-JP" sz="1100"/>
+            <a:t>Secure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>WebView</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>を起動</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2229A4C8-B2D3-CB4A-A677-033FB0D1ADB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8750300" y="1206500"/>
+          <a:ext cx="406400" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>203708</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Circular Arrow 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E0AEE5E-BEFE-4341-93CC-19EC9DE76DB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="13002414">
+          <a:off x="11607800" y="7696199"/>
+          <a:ext cx="978408" cy="2616200"/>
+        </a:xfrm>
+        <a:prstGeom prst="circularArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 3017"/>
+            <a:gd name="adj2" fmla="val 1142319"/>
+            <a:gd name="adj3" fmla="val 20807551"/>
+            <a:gd name="adj4" fmla="val 10800000"/>
+            <a:gd name="adj5" fmla="val 11809"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Rectangle 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{636A5F8C-A463-344A-8516-CBA6B427287B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22771100" y="927100"/>
+          <a:ext cx="2120900" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>&lt;App&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>画面を表示</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>63501</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE02FB6-C33B-264A-9AD7-73FEAC99C296}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="18643600" y="5981700"/>
+          <a:ext cx="812800" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>179173</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="83" name="Group 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47AF53FD-39EC-B141-AE96-6203462C1B4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11798300" y="2946400"/>
+          <a:ext cx="3822700" cy="6198973"/>
+          <a:chOff x="19050000" y="2946400"/>
+          <a:chExt cx="3822700" cy="6198973"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="22" name="Picture 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2453563A-3B10-7B4B-8CFB-C3DB23E723A4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19050000" y="2946400"/>
+            <a:ext cx="3822700" cy="6198973"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="23" name="Picture 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48C5EF7D-72C9-1948-80F8-A801688F4FA3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19392900" y="3492500"/>
+            <a:ext cx="2859249" cy="4953000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32798CE7-68E7-0A40-A89D-7D3A2592EB52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20993100" y="5969000"/>
+          <a:ext cx="2349500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Rounded Rectangle 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F299C930-782F-BE48-93C5-680D8294832F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10731500" y="10401300"/>
+          <a:ext cx="2997200" cy="673100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            <a:t>app.js: App Login Screen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            <a:t>appLogin.ejs</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>39473</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="79" name="Group 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC270421-D485-7343-8B18-BF0AE02BE3A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="15684500" y="3009900"/>
+          <a:ext cx="3683000" cy="6198973"/>
+          <a:chOff x="24625300" y="3009900"/>
+          <a:chExt cx="3822700" cy="6198973"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="43" name="Group 42">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4CB76B0-0EE6-A947-A4D7-FDC995E4898C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="24625300" y="3009900"/>
+            <a:ext cx="3822700" cy="6198973"/>
+            <a:chOff x="24625300" y="3009900"/>
+            <a:chExt cx="3822700" cy="6198973"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="44" name="Group 43">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29A76286-03C2-0B4D-B43F-276F0DF95281}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="24625300" y="3009900"/>
+              <a:ext cx="3822700" cy="6198973"/>
+              <a:chOff x="22771100" y="2921000"/>
+              <a:chExt cx="3822700" cy="6198973"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="47" name="Picture 46">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E4E2C7-03AB-044F-B4E6-30A7F6CA3F08}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="22771100" y="2921000"/>
+                <a:ext cx="3822700" cy="6198973"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="48" name="Picture 47">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AFE5C40-3839-EF4B-892E-8050844475C5}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="23114000" y="3492500"/>
+                <a:ext cx="2853626" cy="4965700"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+          <xdr:pic>
+            <xdr:nvPicPr>
+              <xdr:cNvPr id="49" name="Picture 48">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5476625A-D8FA-F145-885C-5863D936BAD8}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvPicPr>
+                <a:picLocks noChangeAspect="1"/>
+              </xdr:cNvPicPr>
+            </xdr:nvPicPr>
+            <xdr:blipFill>
+              <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+              <a:stretch>
+                <a:fillRect/>
+              </a:stretch>
+            </xdr:blipFill>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="23139400" y="3733800"/>
+                <a:ext cx="2743200" cy="4826978"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+            </xdr:spPr>
+          </xdr:pic>
+        </xdr:grpSp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="45" name="Picture 44">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253005A3-2807-3541-8EF3-D5A416808CB2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm flipV="1">
+              <a:off x="27292300" y="6019800"/>
+              <a:ext cx="444500" cy="444500"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="46" name="Picture 45">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A5E9CA4-9F71-FB43-9069-D51D5870832B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm flipV="1">
+              <a:off x="25006300" y="6070600"/>
+              <a:ext cx="444500" cy="444500"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </xdr:grpSp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="77" name="Picture 76">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B599303-2E85-D14A-98D2-AFD09FE55243}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="26212800" y="3619500"/>
+            <a:ext cx="482600" cy="241300"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="Rounded Rectangular Callout 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED212CAB-DACD-C645-B985-5A319D9E2C99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2298700" y="6997700"/>
+          <a:ext cx="1638300" cy="1079500"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 68562"/>
+            <a:gd name="adj2" fmla="val 129293"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>Appから渡されたtokenを、Cookieに設定</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C3F2481-EBED-5D48-94CC-A94D68E38EEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="17386300" y="1460500"/>
+          <a:ext cx="1231900" cy="3771900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="Rounded Rectangular Callout 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3BD8247-1BCD-4642-8D9F-2905CF2550E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11772900" y="10096500"/>
+          <a:ext cx="2298700" cy="939800"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -71950"/>
+            <a:gd name="adj2" fmla="val 2520"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>checkoutReviewReturnUrlには「/static/next.html」を指定</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="82" name="Rounded Rectangular Callout 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32CA683C-EA75-824A-894B-796A3A6FF738}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15748000" y="2489200"/>
+          <a:ext cx="1549400" cy="1079500"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 57907"/>
+            <a:gd name="adj2" fmla="val 192820"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>CookieのtokenをURLパラメタとして付与</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4897,9 +6246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCEA858D-4327-E246-AC75-10AD98E76650}">
   <dimension ref="B1:BE58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8274,4 +9621,1551 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED98987-2D8D-AA4B-B624-4AAC5B5EB1D1}">
+  <dimension ref="B1:Y58"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B2" s="13"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="4"/>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B3" s="15"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="6"/>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="6"/>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="6"/>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="6"/>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B10" s="15"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="6"/>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B12" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="6"/>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="6"/>
+    </row>
+    <row r="14" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="11"/>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B15" s="13"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="4"/>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="6"/>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B17" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="6"/>
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B18" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="6"/>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B19" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="6"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="6"/>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B21" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="6"/>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="6"/>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B23" s="15"/>
+      <c r="C23" s="7"/>
+      <c r="E23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="6"/>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B24" s="15"/>
+      <c r="C24" s="7"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="6"/>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B25" s="15"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="6"/>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B26" s="15"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="6"/>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B27" s="15"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="6"/>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B28" s="15"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="6"/>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B29" s="15"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="6"/>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B30" s="15"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="6"/>
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B31" s="15"/>
+      <c r="C31" s="7"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="6"/>
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B32" s="15"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="6"/>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B33" s="15"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="6"/>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B34" s="15"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="6"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B35" s="15"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="6"/>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B36" s="15"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="6"/>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B37" s="15"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="6"/>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B38" s="15"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="5"/>
+      <c r="W38" s="5"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="6"/>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B39" s="15"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39" s="5"/>
+      <c r="W39" s="5"/>
+      <c r="X39" s="5"/>
+      <c r="Y39" s="6"/>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B40" s="15"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="6"/>
+    </row>
+    <row r="41" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B41" s="15"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="6"/>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B42" s="15"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="6"/>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B43" s="15"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="5"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="6"/>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B44" s="15"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="6"/>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B45" s="15"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="6"/>
+    </row>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B46" s="15"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="6"/>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B47" s="15"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="6"/>
+    </row>
+    <row r="48" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="16"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
+      <c r="S48" s="10"/>
+      <c r="T48" s="10"/>
+      <c r="U48" s="10"/>
+      <c r="V48" s="10"/>
+      <c r="W48" s="10"/>
+      <c r="X48" s="10"/>
+      <c r="Y48" s="11"/>
+    </row>
+    <row r="49" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B49" s="13"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="18"/>
+      <c r="W49" s="18"/>
+      <c r="X49" s="18"/>
+      <c r="Y49" s="4"/>
+    </row>
+    <row r="50" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B50" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="5"/>
+      <c r="Y50" s="6"/>
+    </row>
+    <row r="51" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B51" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="Y51" s="6"/>
+    </row>
+    <row r="52" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B52" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
+      <c r="V52" s="5"/>
+      <c r="W52" s="5"/>
+      <c r="X52" s="5"/>
+      <c r="Y52" s="6"/>
+    </row>
+    <row r="53" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B53" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="7"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="6"/>
+    </row>
+    <row r="54" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B54" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="6"/>
+    </row>
+    <row r="55" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B55" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="5"/>
+      <c r="T55" s="5"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="6"/>
+    </row>
+    <row r="56" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B56" s="15"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
+      <c r="Y56" s="6"/>
+    </row>
+    <row r="57" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B57" s="15"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="5"/>
+      <c r="T57" s="5"/>
+      <c r="U57" s="5"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="5"/>
+      <c r="Y57" s="6"/>
+    </row>
+    <row r="58" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="16"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
+      <c r="N58" s="10"/>
+      <c r="O58" s="10"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
+      <c r="R58" s="10"/>
+      <c r="S58" s="10"/>
+      <c r="T58" s="10"/>
+      <c r="U58" s="10"/>
+      <c r="V58" s="10"/>
+      <c r="W58" s="10"/>
+      <c r="X58" s="10"/>
+      <c r="Y58" s="11"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E50" r:id="rId1" xr:uid="{D7D2F198-D545-964E-9477-C889B1041F4D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>